<commit_message>
Day 3 Zig Zag
</commit_message>
<xml_diff>
--- a/Python cheet sheet.xlsx
+++ b/Python cheet sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a955fc45c1aa0037/Documentos/Hacker Rank/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="152" documentId="8_{A6DB17BF-B560-47FF-B265-6F0D11B51429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{085FB762-EFA0-4DD2-A504-97AF3270B91C}"/>
+  <xr:revisionPtr revIDLastSave="158" documentId="8_{A6DB17BF-B560-47FF-B265-6F0D11B51429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDC8F65D-1BB1-4880-8453-56C8AB247077}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{CE74CF26-60C0-4E25-B80B-4BF3E894889E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CE74CF26-60C0-4E25-B80B-4BF3E894889E}"/>
   </bookViews>
   <sheets>
     <sheet name="Operators" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>range</t>
   </si>
@@ -274,6 +274,16 @@
 finally:
 	#and finally here
     print("Have a good day")</t>
+  </si>
+  <si>
+    <t>print("Welcome to" , end = ' ') 
+print("GeeksforGeeks", end = ' ')</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># ends the output with a &lt;space&gt; </t>
+  </si>
+  <si>
+    <t>Welcome to GeeksforGeeks</t>
   </si>
 </sst>
 </file>
@@ -755,15 +765,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F15BDCB-59CD-4013-B565-61EA9625A827}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.77734375" customWidth="1"/>
+    <col min="1" max="1" width="30.44140625" customWidth="1"/>
     <col min="2" max="2" width="75.88671875" customWidth="1"/>
     <col min="3" max="3" width="60.77734375" customWidth="1"/>
   </cols>
@@ -902,12 +912,23 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>60</v>
       </c>
       <c r="B17" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -953,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D25972CB-1E43-064D-8FED-1AB7EFD92163}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>